<commit_message>
Updated the code for Keyword Driven
</commit_message>
<xml_diff>
--- a/uclidmmp/keywordData.xlsx
+++ b/uclidmmp/keywordData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sudhe\git\plutogit\mmppluto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sudhe\git\seleniumrepouclid\uclidmmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28579194-0394-427D-9609-954F7BEF98F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04D0EEB-374F-4469-8473-805C5A8CFF51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
   <si>
     <t>Description</t>
   </si>
@@ -116,12 +116,19 @@
   </si>
   <si>
     <t>Result</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -619,16 +626,16 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:F3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.54296875" style="3" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.08984375" style="3" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.81640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" style="3" width="16.54296875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="15.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="18.81640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="22.08984375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="3" width="11.81640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
@@ -778,6 +785,9 @@
       <c r="F7" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="G7" t="s" s="0">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
@@ -881,6 +891,9 @@
       </c>
       <c r="F12" s="7" t="s">
         <v>27</v>
+      </c>
+      <c r="G12" t="s" s="0">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding new testcase E2E_002
</commit_message>
<xml_diff>
--- a/uclidmmp/keywordData.xlsx
+++ b/uclidmmp/keywordData.xlsx
@@ -1,29 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sudhe\git\seleniumrepouclid\uclidmmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04D0EEB-374F-4469-8473-805C5A8CFF51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5B9533-38B6-4D76-8726-7A4DC79C7E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="E2E_001" sheetId="1" r:id="rId1"/>
+    <sheet name="E2E_002" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">E2E_001!$A$1:$G$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">E2E_002!$A$1:$G$6</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="42">
   <si>
     <t>Description</t>
   </si>
@@ -118,17 +120,43 @@
     <t>Result</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>http://96.84.175.78/MMP-Release2-Integrated-Build.6.8.000/portal/login.php</t>
+  </si>
+  <si>
+    <t>Ria12345</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>submit</t>
+  </si>
+  <si>
+    <t>Submit Button</t>
+  </si>
+  <si>
+    <t>ria12345</t>
+  </si>
+  <si>
+    <t>verifyTextInAlert</t>
+  </si>
+  <si>
+    <t>Wrong username and password.</t>
+  </si>
+  <si>
+    <t>Launch MMP Application</t>
+  </si>
+  <si>
+    <t>ria1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -272,7 +300,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -317,6 +345,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -625,17 +656,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" customWidth="true" style="3" width="16.54296875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="15.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="18.81640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="22.08984375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="3" width="11.81640625" collapsed="true"/>
+    <col min="2" max="2" width="16.54296875" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.08984375" style="3" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.81640625" style="3" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
@@ -785,8 +816,8 @@
       <c r="F7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G7" t="s" s="0">
-        <v>32</v>
+      <c r="G7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -892,8 +923,8 @@
       <c r="F12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G12" t="s" s="0">
-        <v>32</v>
+      <c r="G12" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -903,4 +934,245 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AAEB76C-7ED7-4DDB-9066-4EA2F3FC9868}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="16.54296875" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.36328125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="36.7265625" style="3" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.81640625" style="3" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="15"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="13">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="15"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="15"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="13">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="1:7" ht="39.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="12">
+        <v>1</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="15"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="13">
+        <v>2</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="15"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="12">
+        <v>3</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="15"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="13">
+        <v>4</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="8"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{58FE9DF9-9C09-429B-9C28-40D4E519DBB0}"/>
+    <hyperlink ref="E7" r:id="rId2" xr:uid="{AF85D283-172E-437B-B8CA-61507B782152}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>